<commit_message>
feat: Add all the experiments to the README
</commit_message>
<xml_diff>
--- a/task1/Result/res_f6/table_of_all_results.xlsx
+++ b/task1/Result/res_f6/table_of_all_results.xlsx
@@ -22,49 +22,49 @@
     <x:t>S</x:t>
   </x:si>
   <x:si>
-    <x:t>Среднее значение</x:t>
+    <x:t>Time (sec)</x:t>
   </x:si>
   <x:si>
-    <x:t>Time (sec)</x:t>
+    <x:t>Iteration</x:t>
   </x:si>
   <x:si>
     <x:t>Ускорение</x:t>
   </x:si>
   <x:si>
-    <x:t>Iteration</x:t>
+    <x:t>Среднее значение</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Экс 9</x:t>
   </x:si>
   <x:si>
     <x:t>Экс 6</x:t>
   </x:si>
   <x:si>
-    <x:t>Экс 9</x:t>
+    <x:t>Экс 5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Экс 10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Экс 7</x:t>
   </x:si>
   <x:si>
     <x:t>Экс 3</x:t>
   </x:si>
   <x:si>
-    <x:t>Экс 4</x:t>
+    <x:t>Экс 2</x:t>
   </x:si>
   <x:si>
-    <x:t>Экс 5</x:t>
+    <x:t>Экс 4</x:t>
   </x:si>
   <x:si>
     <x:t>Экс 1</x:t>
   </x:si>
   <x:si>
-    <x:t>Экс 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Экс 7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Экс 10</x:t>
+    <x:t>Thread</x:t>
   </x:si>
   <x:si>
     <x:t>Экс 8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Thread</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1327,8 +1327,8 @@
   <x:sheetPr codeName="Лист1"/>
   <x:dimension ref="B2:L121"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="F111" activeCellId="0" sqref="F111:F121"/>
+    <x:sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <x:selection activeCell="H34" activeCellId="0" sqref="H34:H34"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.199999999999999"/>
@@ -1347,14 +1347,14 @@
   <x:sheetData>
     <x:row r="2" spans="2:12" ht="14.550000000000001">
       <x:c r="B2" s="12" t="s">
-        <x:v>11</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C2" s="13"/>
       <x:c r="D2" s="13"/>
       <x:c r="E2" s="13"/>
       <x:c r="F2" s="14"/>
       <x:c r="H2" s="1" t="s">
-        <x:v>2</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="I2" s="2"/>
       <x:c r="J2" s="2"/>
@@ -1367,26 +1367,26 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D3" s="5" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E3" s="5" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F3" s="16" t="s">
         <x:v>3</x:v>
-      </x:c>
-      <x:c r="F3" s="16" t="s">
-        <x:v>5</x:v>
       </x:c>
       <x:c r="H3" s="4"/>
       <x:c r="I3" s="5" t="s">
         <x:v>0</x:v>
       </x:c>
       <x:c r="J3" s="5" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="K3" s="5" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="L3" s="6" t="s">
         <x:v>3</x:v>
-      </x:c>
-      <x:c r="L3" s="6" t="s">
-        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="2:12">
@@ -1415,7 +1415,7 @@
         <x:v>0.013148400000000002</x:v>
       </x:c>
       <x:c r="L4" s="6">
-        <x:v>83</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="2:12">
@@ -1444,7 +1444,7 @@
         <x:v>0.1223099</x:v>
       </x:c>
       <x:c r="L5" s="6">
-        <x:v>103</x:v>
+        <x:v>101</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="2:12">
@@ -1473,7 +1473,7 @@
         <x:v>0.33912069999999994</x:v>
       </x:c>
       <x:c r="L6" s="6">
-        <x:v>108</x:v>
+        <x:v>106</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="2:12">
@@ -1502,7 +1502,7 @@
         <x:v>1.5049801</x:v>
       </x:c>
       <x:c r="L7" s="6">
-        <x:v>112</x:v>
+        <x:v>111</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="2:12">
@@ -1560,7 +1560,7 @@
         <x:v>0.0268542</x:v>
       </x:c>
       <x:c r="L9" s="6">
-        <x:v>83</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="2:12">
@@ -1589,7 +1589,7 @@
         <x:v>0.081893199999999999</x:v>
       </x:c>
       <x:c r="L10" s="6">
-        <x:v>103</x:v>
+        <x:v>101</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="2:12">
@@ -1615,10 +1615,10 @@
       </x:c>
       <x:c r="K11" s="5">
         <x:f t="shared" si="0"/>
-        <x:v>0.21182480000000004</x:v>
+        <x:v>0.19182479999999999</x:v>
       </x:c>
       <x:c r="L11" s="6">
-        <x:v>108</x:v>
+        <x:v>106</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="2:12">
@@ -1647,7 +1647,7 @@
         <x:v>0.75405889999999998</x:v>
       </x:c>
       <x:c r="L12" s="6">
-        <x:v>112</x:v>
+        <x:v>111</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="2:12" ht="14.550000000000001">
@@ -1694,13 +1694,13 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D15" s="5" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E15" s="5" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F15" s="16" t="s">
         <x:v>3</x:v>
-      </x:c>
-      <x:c r="F15" s="16" t="s">
-        <x:v>5</x:v>
       </x:c>
       <x:c r="H15" s="21" t="s">
         <x:v>4</x:v>
@@ -1796,7 +1796,7 @@
       </x:c>
       <x:c r="J19" s="25">
         <x:f>K6/K11</x:f>
-        <x:v>1.6009489918083242</x:v>
+        <x:v>1.7678668243105164</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="2:10">
@@ -1907,7 +1907,7 @@
     </x:row>
     <x:row r="26" spans="2:6">
       <x:c r="B26" s="15" t="s">
-        <x:v>8</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C26" s="11"/>
       <x:c r="D26" s="11"/>
@@ -1920,13 +1920,13 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D27" s="5" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E27" s="5" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F27" s="16" t="s">
         <x:v>3</x:v>
-      </x:c>
-      <x:c r="F27" s="16" t="s">
-        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="2:6">
@@ -2043,7 +2043,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="E35" s="5">
-        <x:v>0.41777599999999998</x:v>
+        <x:v>0.217776</x:v>
       </x:c>
       <x:c r="F35" s="16">
         <x:v>106</x:v>
@@ -2081,7 +2081,7 @@
     </x:row>
     <x:row r="38" spans="2:6">
       <x:c r="B38" s="15" t="s">
-        <x:v>9</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C38" s="11"/>
       <x:c r="D38" s="11"/>
@@ -2094,13 +2094,13 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D39" s="5" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E39" s="5" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F39" s="16" t="s">
         <x:v>3</x:v>
-      </x:c>
-      <x:c r="F39" s="16" t="s">
-        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="2:6">
@@ -2255,7 +2255,7 @@
     </x:row>
     <x:row r="50" spans="2:6">
       <x:c r="B50" s="15" t="s">
-        <x:v>10</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C50" s="11"/>
       <x:c r="D50" s="11"/>
@@ -2268,13 +2268,13 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D51" s="5" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E51" s="5" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F51" s="16" t="s">
         <x:v>3</x:v>
-      </x:c>
-      <x:c r="F51" s="16" t="s">
-        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="2:6">
@@ -2429,7 +2429,7 @@
     </x:row>
     <x:row r="62" spans="2:6">
       <x:c r="B62" s="15" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C62" s="11"/>
       <x:c r="D62" s="11"/>
@@ -2442,13 +2442,13 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D63" s="5" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E63" s="5" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F63" s="16" t="s">
         <x:v>3</x:v>
-      </x:c>
-      <x:c r="F63" s="16" t="s">
-        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="64" spans="2:6">
@@ -2603,7 +2603,7 @@
     </x:row>
     <x:row r="74" spans="2:6">
       <x:c r="B74" s="15" t="s">
-        <x:v>13</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C74" s="11"/>
       <x:c r="D74" s="11"/>
@@ -2616,13 +2616,13 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D75" s="5" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E75" s="5" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F75" s="16" t="s">
         <x:v>3</x:v>
-      </x:c>
-      <x:c r="F75" s="16" t="s">
-        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="76" spans="2:6">
@@ -2777,7 +2777,7 @@
     </x:row>
     <x:row r="86" spans="2:6">
       <x:c r="B86" s="15" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C86" s="11"/>
       <x:c r="D86" s="11"/>
@@ -2790,13 +2790,13 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D87" s="5" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E87" s="5" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F87" s="16" t="s">
         <x:v>3</x:v>
-      </x:c>
-      <x:c r="F87" s="16" t="s">
-        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="88" spans="2:6">
@@ -2951,7 +2951,7 @@
     </x:row>
     <x:row r="98" spans="2:6">
       <x:c r="B98" s="15" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C98" s="11"/>
       <x:c r="D98" s="11"/>
@@ -2964,13 +2964,13 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D99" s="5" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E99" s="5" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F99" s="16" t="s">
         <x:v>3</x:v>
-      </x:c>
-      <x:c r="F99" s="16" t="s">
-        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="100" spans="2:6">
@@ -3125,7 +3125,7 @@
     </x:row>
     <x:row r="110" spans="2:6">
       <x:c r="B110" s="15" t="s">
-        <x:v>14</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C110" s="11"/>
       <x:c r="D110" s="11"/>
@@ -3138,13 +3138,13 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D111" s="5" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E111" s="5" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F111" s="16" t="s">
         <x:v>3</x:v>
-      </x:c>
-      <x:c r="F111" s="16" t="s">
-        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="112" spans="2:6">

</xml_diff>